<commit_message>
Commit 7 added new script to testng.xml
</commit_message>
<xml_diff>
--- a/result/result.xlsx
+++ b/result/result.xlsx
@@ -2,21 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView windowHeight="8010" windowWidth="14805" xWindow="240" yWindow="105"/>
   </bookViews>
   <sheets>
-    <sheet name="Result" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Result" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet2" r:id="rId2" sheetId="2"/>
+    <sheet name="Sheet3" r:id="rId3" sheetId="3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -28,12 +28,34 @@
   </si>
   <si>
     <t>Browser</t>
+  </si>
+  <si>
+    <t>testMultipleLogin</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>01_03_2017_01_08_52</t>
+  </si>
+  <si>
+    <t>CHROME</t>
+  </si>
+  <si>
+    <t>01_03_2017_01_08_59</t>
+  </si>
+  <si>
+    <t>testLoginLogout</t>
+  </si>
+  <si>
+    <t>01_03_2017_01_09_14</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -70,19 +92,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -96,10 +118,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -257,7 +279,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -266,13 +288,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -282,7 +304,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -291,7 +313,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -300,7 +322,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -310,12 +332,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -346,7 +368,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -365,7 +387,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -377,17 +399,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="19.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -404,32 +426,74 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>